<commit_message>
silly change for an example
</commit_message>
<xml_diff>
--- a/Working Documents/MARC2RDA Bibliographic Map Errors.xlsx
+++ b/Working Documents/MARC2RDA Bibliographic Map Errors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/cec23_uw_edu/Documents/Documents/Metadata/Linked Data Projects/MARC2RDA/Working Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49C62FEB-F864-44B8-BF08-A44F558B2AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{49C62FEB-F864-44B8-BF08-A44F558B2AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63748E3D-F521-401B-A95C-E8FEBCA9DF0E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="99">
   <si>
-    <t>RDA Registry mapping</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>776 ** $f does not exist</t>
+  </si>
+  <si>
+    <t>RDA Registry mapping (original from RSC)</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -634,761 +634,761 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="C20" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="C23" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="C24" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C25" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="C28" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="C29" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="C32" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="C35" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="C42" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="C44" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="C50" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="C52" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="C54" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="C56" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="C58" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="C64" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B65" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C65" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B67" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="C68" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>